<commit_message>
update FTDI caravel board PCB and BOM (Rev 3C)
</commit_message>
<xml_diff>
--- a/hardware/caravel_pcb_v3_FTDI/caravel_pcb_v3_FTDI.xlsx
+++ b/hardware/caravel_pcb_v3_FTDI/caravel_pcb_v3_FTDI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Efabless\caravel_board\hardware\caravel_pcb_v3_FTDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DED6CE-FB42-4E61-9943-B94A7C33E1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5F35BB-A34F-427D-AAB8-3F18E5FDBD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
+    <workbookView xWindow="2960" yWindow="2960" windowWidth="19200" windowHeight="11170" xr2:uid="{DBB590BE-7B6D-5543-BF5E-2321E179B520}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>U6</t>
   </si>
@@ -60,15 +60,9 @@
     <t>U4</t>
   </si>
   <si>
-    <t>R11</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
-    <t>D1, D2, D3</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>C9, C10, C11, C12</t>
-  </si>
-  <si>
     <t>C13, C14, C18, C19</t>
   </si>
   <si>
@@ -214,6 +205,21 @@
   </si>
   <si>
     <t>LDI1117-3.3H</t>
+  </si>
+  <si>
+    <t>C9-C12</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4</t>
+  </si>
+  <si>
+    <t>R11, R14</t>
+  </si>
+  <si>
+    <t>TP1, TP2</t>
+  </si>
+  <si>
+    <t>36-5000-ND</t>
   </si>
 </sst>
 </file>
@@ -300,7 +306,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -326,9 +332,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -647,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718CFFD5-71E2-E44C-BCD6-97EE3DEEFA9F}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -663,19 +666,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -687,28 +690,28 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -723,29 +726,29 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>19</v>
+        <v>56</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -760,178 +763,178 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B8" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B9" s="7">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B10" s="7">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B11" s="7">
         <v>2</v>
       </c>
       <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>24</v>
-      </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B12" s="7">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B13" s="7">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="7">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" s="7">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="7">
         <v>2</v>
@@ -940,27 +943,27 @@
         <v>150</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B18" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="4">
         <v>82</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -971,10 +974,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -985,13 +988,13 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1002,13 +1005,27 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="7">
+        <v>2</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1032,8 +1049,9 @@
     <hyperlink ref="D21" r:id="rId17" xr:uid="{1F484673-4C77-4CD6-8F13-F5756E1F14E9}"/>
     <hyperlink ref="D5" r:id="rId18" xr:uid="{AC4A8384-9698-417E-B845-F4D6E4DAD7D2}"/>
     <hyperlink ref="G5" r:id="rId19" xr:uid="{D63976FF-547D-46FE-8D03-6E293B2A60F9}"/>
+    <hyperlink ref="D22" r:id="rId20" xr:uid="{77AF3B6F-44B4-4877-A203-88B8BD419D7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>